<commit_message>
All functions are included, data is still a problem
</commit_message>
<xml_diff>
--- a/Model_Version3/Data/model_input_data_891.xlsx
+++ b/Model_Version3/Data/model_input_data_891.xlsx
@@ -12,12 +12,12 @@
     <sheet name="Dissabilities" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Education_level" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Percent_working_per_age" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sector_distribution" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Occupation_and_employment" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Land_sizes" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Work_type_per_land_size" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Expenditure_per_hh_member" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Member_association" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Land_sizes" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Work_type_per_land_size" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Expenditure_per_hh_member" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Member_association" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Sector_distribution" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Occupation_and_employment" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Experience_per_occupation" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Statistics_population_size" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Housing_quality" sheetId="14" state="visible" r:id="rId14"/>
@@ -532,7 +532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,43 +543,63 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Percentile</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Yearly_expenditure_per_member</t>
+          <t>Probability</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>Non_agri</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1755.6</v>
+        <v>0.5667236374487942</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2599</v>
+        <v>0.3830064295596972</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>Annual crops</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4019</v>
+        <v>0.0331786983532731</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Perennial crops</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.01600607688342693</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Aquaculture</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.001085157754808605</v>
       </c>
     </row>
   </sheetData>
@@ -593,7 +613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,33 +624,369 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Association</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Percentage</t>
+          <t>Occupation</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Family_worker</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>perc_occupation</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.8829376035339591</v>
+          <t>Annual crops</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>low_skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>52.08503679476697</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.1170623964660409</v>
+          <t>Annual crops</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>47.91496320523304</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Aquaculture</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>low_skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Aquaculture</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Non_agri</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>low_skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>98.3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.814743896601245</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Non_agri</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>low_skilled_nonAgri</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>93.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>19.06175203446625</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Non_agri</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>manual_worker</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>85.5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11.05313547151747</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Non_agri</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>91</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13.28386787936812</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Non_agri</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>skilled_service_worker</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>53.78650071804692</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Perennial crops</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>low_skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="D11" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>40.84745762711864</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Perennial crops</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>65</v>
+      </c>
+      <c r="D12" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="F12" t="n">
+        <v>59.15254237288136</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>low_skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>96.09999999999999</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>31.27921801954951</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>manual_worker</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>100</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.06374840628984275</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>skilled_agri_worker</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>51.8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>43.7</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="F15" t="n">
+        <v>68.65703357416064</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1590,63 +1946,43 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>land_size_type</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>percentage</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Other agriculture</t>
+          <t>small</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7166798449462904</v>
+        <v>0.5605435573889832</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Non_agri</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2642470059591537</v>
+        <v>0.3734530453773356</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Perennial crops</t>
+          <t>large</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01575607968680693</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Aquaculture</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.003317069407748828</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Annual crops</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
+        <v>0.06600339723368115</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1671,393 +2007,622 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>Dominant_income_source</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Occupation</t>
+          <t>land_size_type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Family_worker</t>
+          <t>Worked_wage</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Employee</t>
+          <t>Worked_self_agri</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>perc_occupation</t>
+          <t>Worked_self_nonAgri</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aquaculture</t>
+          <t>Annual crops</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>low_skilled_agri_worker</t>
+          <t>small</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>76.09999999999999</v>
+        <v>0.9380530973451328</v>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>1.929203539823009</v>
       </c>
       <c r="E2" t="n">
-        <v>14.9</v>
-      </c>
-      <c r="F2" t="n">
-        <v>38.95348837209303</v>
+        <v>0.1327433628318584</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Aquaculture</t>
+          <t>Annual crops</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>skilled_agri_worker</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="D3" t="n">
-        <v>4.8</v>
+        <v>2.469135802469136</v>
       </c>
       <c r="E3" t="n">
-        <v>95.2</v>
-      </c>
-      <c r="F3" t="n">
-        <v>61.04651162790697</v>
+        <v>0.1604938271604938</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Non_agri</t>
+          <t>Annual crops</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>low_skilled_agri_worker</t>
+          <t>large</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>80.90000000000001</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5.948036782951394</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Non_agri</t>
+          <t>Aquaculture</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>low_skilled_nonAgri</t>
+          <t>small</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6.1</v>
+        <v>0.6373626373626373</v>
       </c>
       <c r="D5" t="n">
-        <v>55.9</v>
+        <v>2.340659340659341</v>
       </c>
       <c r="E5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F5" t="n">
-        <v>13.62574806597577</v>
+        <v>0.2307692307692308</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Non_agri</t>
+          <t>Aquaculture</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>manual_worker</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>0.375</v>
       </c>
       <c r="D6" t="n">
-        <v>50.3</v>
+        <v>2.6625</v>
       </c>
       <c r="E6" t="n">
-        <v>46.6</v>
-      </c>
-      <c r="F6" t="n">
-        <v>24.56575682382134</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Non_agri</t>
+          <t>Aquaculture</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>skilled_agri_worker</t>
+          <t>large</t>
         </is>
       </c>
       <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E7" t="n">
-        <v>99.09999999999999</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6.823821339950372</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Non_agri</t>
+          <t>Perennial crops</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>skilled_service_worker</t>
+          <t>small</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.9</v>
+        <v>0.4104973973395026</v>
       </c>
       <c r="D8" t="n">
-        <v>33.9</v>
+        <v>1.70655002891845</v>
       </c>
       <c r="E8" t="n">
-        <v>61.1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>49.03663698730112</v>
+        <v>0.143796992481203</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Other agriculture</t>
+          <t>Perennial crops</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>low_skilled_agri_worker</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>26.2</v>
+        <v>0.7192040772066797</v>
       </c>
       <c r="D9" t="n">
-        <v>72</v>
+        <v>2.100683148991542</v>
       </c>
       <c r="E9" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="F9" t="n">
-        <v>57.86287067434476</v>
+        <v>0.2375840381695944</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Other agriculture</t>
+          <t>Perennial crops</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>low_skilled_nonAgri</t>
+          <t>large</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.6545454545454545</v>
       </c>
       <c r="D10" t="n">
-        <v>94</v>
+        <v>2.572727272727273</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.180291695818309</v>
+        <v>0.1863636363636363</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Other agriculture</t>
+          <t>Revenue_by_products</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>manual_worker</t>
+          <t>small</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.0269092083310909</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Other agriculture</t>
+          <t>Revenue_by_products</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>skilled_agri_worker</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>99.5</v>
-      </c>
-      <c r="F12" t="n">
-        <v>41.87880092567677</v>
+          <t>medium</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Other agriculture</t>
+          <t>Revenue_by_products</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>skilled_service_worker</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>100</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.05112749582907271</v>
+          <t>large</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Perennial crops</t>
+          <t>Revenue_hunting_etc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>low_skilled_agri_worker</t>
+          <t>small</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>57.1</v>
+        <v>0.7325581395348837</v>
       </c>
       <c r="D14" t="n">
-        <v>42.9</v>
+        <v>2.052325581395349</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>35.12851897184823</v>
+        <v>0.3488372093023256</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Perennial crops</t>
+          <t>Revenue_hunting_etc</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>skilled_agri_worker</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0.6627906976744186</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>2.465116279069767</v>
       </c>
       <c r="E15" t="n">
-        <v>99</v>
-      </c>
-      <c r="F15" t="n">
-        <v>64.38188494492044</v>
+        <v>0.3488372093023256</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Perennial crops</t>
+          <t>Revenue_hunting_etc</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>skilled_service_worker</t>
+          <t>large</t>
         </is>
       </c>
       <c r="C16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E16" t="n">
         <v>0</v>
       </c>
-      <c r="D16" t="n">
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Revenue_machines</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>small</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Revenue_machines</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Revenue_machines</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>large</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="E16" t="n">
-        <v>100</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.4895960832313341</v>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Revenue_processing_aqua_agri</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>small</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.5304347826086957</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.602898550724638</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1.617391304347826</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Revenue_processing_aqua_agri</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.4411764705882353</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.950980392156863</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.950980392156863</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Revenue_processing_aqua_agri</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>large</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Revenues_foresty</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>small</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Revenues_foresty</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Revenues_foresty</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>large</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>small</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.9232736572890026</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.864450127877238</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.1585677749360614</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.7503045066991474</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2.269183922046285</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.2789281364190012</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>large</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.4759825327510917</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2.59825327510917</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.3580786026200873</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>wages</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>small</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1.899408284023669</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.757396449704142</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.1644970414201183</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>wages</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2.01875</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2.0875</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>wages</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>large</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2082,43 +2647,43 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>land_size_type</t>
+          <t>Percentile</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>percentage</t>
+          <t>Yearly_expenditure_per_member</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>small</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5605435573889832</v>
+        <v>1755.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>medium</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3734530453773356</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>large</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06600339723368115</v>
+        <v>4019</v>
       </c>
     </row>
   </sheetData>
@@ -2132,7 +2697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2143,622 +2708,33 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Dominant_income_source</t>
+          <t>Association</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>land_size_type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Worked_wage</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Worked_self_agri</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Worked_self_nonAgri</t>
+          <t>Percentage</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Annual crops</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.9380530973451328</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.929203539823009</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.1327433628318584</v>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.8829376035339591</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Annual crops</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.9629629629629629</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.469135802469136</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.1604938271604938</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Annual crops</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Aquaculture</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.6373626373626373</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.340659340659341</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2307692307692308</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Aquaculture</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.6625</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Aquaculture</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Other agriculture</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.9232736572890026</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.864450127877238</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1585677749360614</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Other agriculture</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0.7503045066991474</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2.269183922046285</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.2789281364190012</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Other agriculture</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.4759825327510917</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2.59825327510917</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.3580786026200873</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Perennial crops</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0.4104973973395026</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.70655002891845</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.143796992481203</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Perennial crops</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.7192040772066797</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2.100683148991542</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.2375840381695944</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Perennial crops</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0.6545454545454545</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2.572727272727273</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.1863636363636363</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Revenue_by_products</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Revenue_by_products</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Revenue_by_products</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Revenue_hunting_etc</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.7325581395348837</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2.052325581395349</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.3488372093023256</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Revenue_hunting_etc</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0.6627906976744186</v>
-      </c>
-      <c r="D18" t="n">
-        <v>2.465116279069767</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.3488372093023256</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Revenue_hunting_etc</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Revenue_machines</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2.125</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Revenue_machines</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="D21" t="n">
-        <v>2.125</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Revenue_machines</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D22" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Revenue_processing_aqua_agri</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>0.5304347826086957</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1.602898550724638</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1.617391304347826</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Revenue_processing_aqua_agri</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0.4411764705882353</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1.950980392156863</v>
-      </c>
-      <c r="E24" t="n">
-        <v>1.950980392156863</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Revenue_processing_aqua_agri</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Revenues_foresty</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Revenues_foresty</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Revenues_foresty</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>wages</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>small</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>1.899408284023669</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1.757396449704142</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.1644970414201183</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>wages</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>2.01875</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2.0875</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>wages</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>large</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1170623964660409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>